<commit_message>
test ETL from oracle collisions table to fusion
</commit_message>
<xml_diff>
--- a/supplementary/column_mapping_btw_analytics_and_oracle_tables.xlsx
+++ b/supplementary/column_mapping_btw_analytics_and_oracle_tables.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="397" documentId="8_{23D0BAB7-18E8-4959-9F4E-FFA96A3ED94C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A9AC5C5-53BE-4AA3-9177-6770C03A6577}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-225" windowWidth="29040" windowHeight="17640" xr2:uid="{FB73D8E5-4A8D-4C49-9DB8-09C218E8D022}"/>
+    <workbookView minimized="1" xWindow="585" yWindow="525" windowWidth="19200" windowHeight="7665" xr2:uid="{FB73D8E5-4A8D-4C49-9DB8-09C218E8D022}"/>
   </bookViews>
   <sheets>
     <sheet name="table - collisions" sheetId="1" r:id="rId1"/>
@@ -1211,6 +1211,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1512,9 +1516,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDB5EC39-7E72-4E02-BEDA-FDADA4B39D58}">
   <dimension ref="A1:N129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K87" sqref="K87"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J46" sqref="J45:J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>